<commit_message>
Fixed where report treating normal notifications as down notifications
</commit_message>
<xml_diff>
--- a/src/AppBundle/tmp/207_server_report.xlsx
+++ b/src/AppBundle/tmp/207_server_report.xlsx
@@ -20,24 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>Date (YYYY/MM/DD)</t>
-  </si>
-  <si>
-    <t>2015-10-17</t>
-  </si>
-  <si>
-    <t>2015-10-18</t>
-  </si>
-  <si>
-    <t>2015-10-19</t>
-  </si>
-  <si>
-    <t>2015-10-20</t>
-  </si>
-  <si>
-    <t>2015-10-21</t>
   </si>
   <si>
     <t>2015-10-22</t>
@@ -244,100 +229,85 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>207_60m_CPU_Avg_!$B$1:$AF$1</c:f>
+              <c:f>207_60m_CPU_Avg_!$B$1:$AA$1</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>2015-10-17</c:v>
+                  <c:v>2015-10-22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2015-10-18</c:v>
+                  <c:v>2015-10-23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2015-10-19</c:v>
+                  <c:v>2015-10-24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2015-10-20</c:v>
+                  <c:v>2015-10-25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2015-10-21</c:v>
+                  <c:v>2015-10-26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2015-10-22</c:v>
+                  <c:v>2015-10-27</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2015-10-23</c:v>
+                  <c:v>2015-10-28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2015-10-24</c:v>
+                  <c:v>2015-10-29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2015-10-25</c:v>
+                  <c:v>2015-10-30</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2015-10-26</c:v>
+                  <c:v>2015-10-31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2015-10-27</c:v>
+                  <c:v>2015-11-01</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2015-10-28</c:v>
+                  <c:v>2015-11-02</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2015-10-29</c:v>
+                  <c:v>2015-11-03</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2015-10-30</c:v>
+                  <c:v>2015-11-04</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2015-10-31</c:v>
+                  <c:v>2015-11-05</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2015-11-01</c:v>
+                  <c:v>2015-11-06</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2015-11-02</c:v>
+                  <c:v>2015-11-07</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2015-11-03</c:v>
+                  <c:v>2015-11-08</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2015-11-04</c:v>
+                  <c:v>2015-11-09</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2015-11-05</c:v>
+                  <c:v>2015-11-10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2015-11-06</c:v>
+                  <c:v>2015-11-11</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2015-11-07</c:v>
+                  <c:v>2015-11-12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2015-11-08</c:v>
+                  <c:v>2015-11-13</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2015-11-09</c:v>
+                  <c:v>2015-11-14</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2015-11-10</c:v>
+                  <c:v>2015-11-15</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2015-11-11</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2015-11-12</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2015-11-13</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2015-11-14</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2015-11-15</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>2015-11-16</c:v>
                 </c:pt>
               </c:strCache>
@@ -345,103 +315,88 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>207_60m_CPU_Avg_!$B$2:$AG$2</c:f>
+              <c:f>207_60m_CPU_Avg_!$B$2:$AB$2</c:f>
               <c:numCache>
-                <c:ptCount val="32"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>1.28</c:v>
+                  <c:v>1.73</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.72</c:v>
+                  <c:v>1.34</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.71</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.88</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.43</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.73</c:v>
+                  <c:v>1.09</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.34</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.09</c:v>
+                  <c:v>0.26</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.22</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.84</c:v>
+                  <c:v>0.31</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.11</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.13</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.26</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.32</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.31</c:v>
+                  <c:v>0.27</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.1</c:v>
+                  <c:v>0.29</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.08</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.1</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.08</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.27</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.29</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.48</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.96</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.95</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.93</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.93</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.04</c:v>
-                </c:pt>
-                <c:pt idx="31">
                   <c:v>1.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -589,9 +544,9 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>207_Memory_Usage!$B$3:$AG$3</c:f>
+              <c:f>207_Memory_Usage!$B$3:$AB$3</c:f>
               <c:numCache>
-                <c:ptCount val="32"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>8345.09</c:v>
                 </c:pt>
@@ -602,10 +557,10 @@
                   <c:v>8345.09</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8345.09</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8345.09</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>8345.09</c:v>
@@ -617,10 +572,10 @@
                   <c:v>8345.09</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-</c:v>
+                  <c:v>8345.09</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-</c:v>
+                  <c:v>8345.09</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>8345.09</c:v>
@@ -671,21 +626,6 @@
                   <c:v>8345.09</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8345.09</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>8345.09</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>8345.09</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>8345.09</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>8345.09</c:v>
-                </c:pt>
-                <c:pt idx="31">
                   <c:v>8345.09</c:v>
                 </c:pt>
               </c:numCache>
@@ -711,100 +651,85 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>207_Memory_Usage!$B$1:$AF$1</c:f>
+              <c:f>207_Memory_Usage!$B$1:$AA$1</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>2015-10-17</c:v>
+                  <c:v>2015-10-22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2015-10-18</c:v>
+                  <c:v>2015-10-23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2015-10-19</c:v>
+                  <c:v>2015-10-24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2015-10-20</c:v>
+                  <c:v>2015-10-25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2015-10-21</c:v>
+                  <c:v>2015-10-26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2015-10-22</c:v>
+                  <c:v>2015-10-27</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2015-10-23</c:v>
+                  <c:v>2015-10-28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2015-10-24</c:v>
+                  <c:v>2015-10-29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2015-10-25</c:v>
+                  <c:v>2015-10-30</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2015-10-26</c:v>
+                  <c:v>2015-10-31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2015-10-27</c:v>
+                  <c:v>2015-11-01</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2015-10-28</c:v>
+                  <c:v>2015-11-02</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2015-10-29</c:v>
+                  <c:v>2015-11-03</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2015-10-30</c:v>
+                  <c:v>2015-11-04</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2015-10-31</c:v>
+                  <c:v>2015-11-05</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2015-11-01</c:v>
+                  <c:v>2015-11-06</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2015-11-02</c:v>
+                  <c:v>2015-11-07</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2015-11-03</c:v>
+                  <c:v>2015-11-08</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2015-11-04</c:v>
+                  <c:v>2015-11-09</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2015-11-05</c:v>
+                  <c:v>2015-11-10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2015-11-06</c:v>
+                  <c:v>2015-11-11</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2015-11-07</c:v>
+                  <c:v>2015-11-12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2015-11-08</c:v>
+                  <c:v>2015-11-13</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2015-11-09</c:v>
+                  <c:v>2015-11-14</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2015-11-10</c:v>
+                  <c:v>2015-11-15</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2015-11-11</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2015-11-12</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2015-11-13</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2015-11-14</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2015-11-15</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>2015-11-16</c:v>
                 </c:pt>
               </c:strCache>
@@ -812,103 +737,88 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>207_Memory_Usage!$B$2:$AG$2</c:f>
+              <c:f>207_Memory_Usage!$B$2:$AB$2</c:f>
               <c:numCache>
-                <c:ptCount val="32"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>3777.41</c:v>
+                  <c:v>3855.54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3785.78</c:v>
+                  <c:v>3859.14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3786.86</c:v>
+                  <c:v>3853.44</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3842.37</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3860.83</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3855.54</c:v>
+                  <c:v>2358.98</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3859.14</c:v>
+                  <c:v>2600.11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3853.44</c:v>
+                  <c:v>2706</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-</c:v>
+                  <c:v>2915.29</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-</c:v>
+                  <c:v>2891.85</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2358.98</c:v>
+                  <c:v>2836.31</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2600.11</c:v>
+                  <c:v>2850.1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2706</c:v>
+                  <c:v>2903.58</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2915.29</c:v>
+                  <c:v>3070.18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2891.85</c:v>
+                  <c:v>3111.38</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2836.31</c:v>
+                  <c:v>3130.37</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2850.1</c:v>
+                  <c:v>3106.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2903.58</c:v>
+                  <c:v>3085.24</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3070.18</c:v>
+                  <c:v>3110.04</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3111.38</c:v>
+                  <c:v>3166.98</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3130.37</c:v>
+                  <c:v>3263.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3106.2</c:v>
+                  <c:v>3103.79</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3085.24</c:v>
+                  <c:v>3069.64</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3110.04</c:v>
+                  <c:v>3067.38</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3166.98</c:v>
+                  <c:v>3034.69</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3263.5</c:v>
+                  <c:v>3045.34</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3103.79</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3069.64</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3067.38</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3034.69</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3045.34</c:v>
-                </c:pt>
-                <c:pt idx="31">
                   <c:v>3109.32</c:v>
                 </c:pt>
               </c:numCache>
@@ -1056,9 +966,9 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>207_C_drive_load!$B$3:$AG$3</c:f>
+              <c:f>207_C_drive_load!$B$3:$AB$3</c:f>
               <c:numCache>
-                <c:ptCount val="32"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>97.3</c:v>
                 </c:pt>
@@ -1069,10 +979,10 @@
                   <c:v>97.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>97.3</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>97.3</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>97.3</c:v>
@@ -1084,10 +994,10 @@
                   <c:v>97.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-</c:v>
+                  <c:v>97.3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-</c:v>
+                  <c:v>97.3</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>97.3</c:v>
@@ -1138,21 +1048,6 @@
                   <c:v>97.3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>97.3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>97.3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>97.3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>97.3</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>97.3</c:v>
-                </c:pt>
-                <c:pt idx="31">
                   <c:v>97.3</c:v>
                 </c:pt>
               </c:numCache>
@@ -1178,100 +1073,85 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>207_C_drive_load!$B$1:$AF$1</c:f>
+              <c:f>207_C_drive_load!$B$1:$AA$1</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>2015-10-17</c:v>
+                  <c:v>2015-10-22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2015-10-18</c:v>
+                  <c:v>2015-10-23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2015-10-19</c:v>
+                  <c:v>2015-10-24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2015-10-20</c:v>
+                  <c:v>2015-10-25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2015-10-21</c:v>
+                  <c:v>2015-10-26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2015-10-22</c:v>
+                  <c:v>2015-10-27</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2015-10-23</c:v>
+                  <c:v>2015-10-28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2015-10-24</c:v>
+                  <c:v>2015-10-29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2015-10-25</c:v>
+                  <c:v>2015-10-30</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2015-10-26</c:v>
+                  <c:v>2015-10-31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2015-10-27</c:v>
+                  <c:v>2015-11-01</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2015-10-28</c:v>
+                  <c:v>2015-11-02</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2015-10-29</c:v>
+                  <c:v>2015-11-03</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2015-10-30</c:v>
+                  <c:v>2015-11-04</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2015-10-31</c:v>
+                  <c:v>2015-11-05</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2015-11-01</c:v>
+                  <c:v>2015-11-06</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2015-11-02</c:v>
+                  <c:v>2015-11-07</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2015-11-03</c:v>
+                  <c:v>2015-11-08</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2015-11-04</c:v>
+                  <c:v>2015-11-09</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2015-11-05</c:v>
+                  <c:v>2015-11-10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2015-11-06</c:v>
+                  <c:v>2015-11-11</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2015-11-07</c:v>
+                  <c:v>2015-11-12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2015-11-08</c:v>
+                  <c:v>2015-11-13</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2015-11-09</c:v>
+                  <c:v>2015-11-14</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2015-11-10</c:v>
+                  <c:v>2015-11-15</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2015-11-11</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2015-11-12</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2015-11-13</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2015-11-14</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2015-11-15</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>2015-11-16</c:v>
                 </c:pt>
               </c:strCache>
@@ -1279,103 +1159,88 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>207_C_drive_load!$B$2:$AG$2</c:f>
+              <c:f>207_C_drive_load!$B$2:$AB$2</c:f>
               <c:numCache>
-                <c:ptCount val="32"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>53.7</c:v>
+                  <c:v>53.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53.61</c:v>
+                  <c:v>53.63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53.6</c:v>
+                  <c:v>53.48</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53.6</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53.62</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53.63</c:v>
+                  <c:v>53.22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53.63</c:v>
+                  <c:v>53.19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53.48</c:v>
+                  <c:v>53.24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-</c:v>
+                  <c:v>53.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-</c:v>
+                  <c:v>53.13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>53.22</c:v>
+                  <c:v>53.13</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53.19</c:v>
+                  <c:v>53.13</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>53.24</c:v>
+                  <c:v>53.13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>53.2</c:v>
+                  <c:v>53.13</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>53.15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>53.05</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>52.98</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>52.98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>52.98</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>52.84</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>53.01</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>53.16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>53.17</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>53.13</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>53.13</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>53.13</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>53.13</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>53.13</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>53.15</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>53.05</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>52.98</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>52.98</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>52.98</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>52.84</c:v>
+                  <c:v>53.08</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>53.01</c:v>
+                  <c:v>53.09</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>53.16</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>53.17</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>53.13</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>53.08</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>53.09</c:v>
-                </c:pt>
-                <c:pt idx="31">
                   <c:v>53.1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1523,9 +1388,9 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>207_E_drive_load!$B$3:$AG$3</c:f>
+              <c:f>207_E_drive_load!$B$3:$AB$3</c:f>
               <c:numCache>
-                <c:ptCount val="32"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>461.43</c:v>
                 </c:pt>
@@ -1536,10 +1401,10 @@
                   <c:v>461.43</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>461.43</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>461.43</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>461.43</c:v>
@@ -1551,10 +1416,10 @@
                   <c:v>461.43</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-</c:v>
+                  <c:v>461.43</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-</c:v>
+                  <c:v>461.43</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>461.43</c:v>
@@ -1605,21 +1470,6 @@
                   <c:v>461.43</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>461.43</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>461.43</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>461.43</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>461.43</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>461.43</c:v>
-                </c:pt>
-                <c:pt idx="31">
                   <c:v>461.43</c:v>
                 </c:pt>
               </c:numCache>
@@ -1645,100 +1495,85 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>207_E_drive_load!$B$1:$AF$1</c:f>
+              <c:f>207_E_drive_load!$B$1:$AA$1</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>2015-10-17</c:v>
+                  <c:v>2015-10-22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2015-10-18</c:v>
+                  <c:v>2015-10-23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2015-10-19</c:v>
+                  <c:v>2015-10-24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2015-10-20</c:v>
+                  <c:v>2015-10-25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2015-10-21</c:v>
+                  <c:v>2015-10-26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2015-10-22</c:v>
+                  <c:v>2015-10-27</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2015-10-23</c:v>
+                  <c:v>2015-10-28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2015-10-24</c:v>
+                  <c:v>2015-10-29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2015-10-25</c:v>
+                  <c:v>2015-10-30</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2015-10-26</c:v>
+                  <c:v>2015-10-31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2015-10-27</c:v>
+                  <c:v>2015-11-01</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2015-10-28</c:v>
+                  <c:v>2015-11-02</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2015-10-29</c:v>
+                  <c:v>2015-11-03</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2015-10-30</c:v>
+                  <c:v>2015-11-04</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2015-10-31</c:v>
+                  <c:v>2015-11-05</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2015-11-01</c:v>
+                  <c:v>2015-11-06</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2015-11-02</c:v>
+                  <c:v>2015-11-07</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2015-11-03</c:v>
+                  <c:v>2015-11-08</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2015-11-04</c:v>
+                  <c:v>2015-11-09</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2015-11-05</c:v>
+                  <c:v>2015-11-10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2015-11-06</c:v>
+                  <c:v>2015-11-11</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2015-11-07</c:v>
+                  <c:v>2015-11-12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2015-11-08</c:v>
+                  <c:v>2015-11-13</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2015-11-09</c:v>
+                  <c:v>2015-11-14</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2015-11-10</c:v>
+                  <c:v>2015-11-15</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2015-11-11</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2015-11-12</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2015-11-13</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2015-11-14</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2015-11-15</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>2015-11-16</c:v>
                 </c:pt>
               </c:strCache>
@@ -1746,9 +1581,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>207_E_drive_load!$B$2:$AG$2</c:f>
+              <c:f>207_E_drive_load!$B$2:$AB$2</c:f>
               <c:numCache>
-                <c:ptCount val="32"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>446.38</c:v>
                 </c:pt>
@@ -1759,10 +1594,10 @@
                   <c:v>446.38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>446.38</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>446.38</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>446.38</c:v>
@@ -1774,10 +1609,10 @@
                   <c:v>446.38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-</c:v>
+                  <c:v>446.38</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-</c:v>
+                  <c:v>446.38</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>446.38</c:v>
@@ -1828,21 +1663,6 @@
                   <c:v>446.38</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>446.38</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>446.38</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>446.38</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>446.38</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>446.38</c:v>
-                </c:pt>
-                <c:pt idx="31">
                   <c:v>446.38</c:v>
                 </c:pt>
               </c:numCache>
@@ -1990,9 +1810,9 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>207_G_drive_load!$B$3:$AG$3</c:f>
+              <c:f>207_G_drive_load!$B$3:$AB$3</c:f>
               <c:numCache>
-                <c:ptCount val="32"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>1117.76</c:v>
                 </c:pt>
@@ -2003,10 +1823,10 @@
                   <c:v>1117.76</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1117.76</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1117.76</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1117.76</c:v>
@@ -2018,10 +1838,10 @@
                   <c:v>1117.76</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-</c:v>
+                  <c:v>1117.76</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-</c:v>
+                  <c:v>1117.76</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1117.76</c:v>
@@ -2072,21 +1892,6 @@
                   <c:v>1117.76</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1117.76</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1117.76</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1117.76</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1117.76</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1117.76</c:v>
-                </c:pt>
-                <c:pt idx="31">
                   <c:v>1117.76</c:v>
                 </c:pt>
               </c:numCache>
@@ -2112,100 +1917,85 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>207_G_drive_load!$B$1:$AF$1</c:f>
+              <c:f>207_G_drive_load!$B$1:$AA$1</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>2015-10-17</c:v>
+                  <c:v>2015-10-22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2015-10-18</c:v>
+                  <c:v>2015-10-23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2015-10-19</c:v>
+                  <c:v>2015-10-24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2015-10-20</c:v>
+                  <c:v>2015-10-25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2015-10-21</c:v>
+                  <c:v>2015-10-26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2015-10-22</c:v>
+                  <c:v>2015-10-27</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2015-10-23</c:v>
+                  <c:v>2015-10-28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2015-10-24</c:v>
+                  <c:v>2015-10-29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2015-10-25</c:v>
+                  <c:v>2015-10-30</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2015-10-26</c:v>
+                  <c:v>2015-10-31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2015-10-27</c:v>
+                  <c:v>2015-11-01</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2015-10-28</c:v>
+                  <c:v>2015-11-02</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2015-10-29</c:v>
+                  <c:v>2015-11-03</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2015-10-30</c:v>
+                  <c:v>2015-11-04</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2015-10-31</c:v>
+                  <c:v>2015-11-05</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2015-11-01</c:v>
+                  <c:v>2015-11-06</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2015-11-02</c:v>
+                  <c:v>2015-11-07</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2015-11-03</c:v>
+                  <c:v>2015-11-08</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2015-11-04</c:v>
+                  <c:v>2015-11-09</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2015-11-05</c:v>
+                  <c:v>2015-11-10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2015-11-06</c:v>
+                  <c:v>2015-11-11</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2015-11-07</c:v>
+                  <c:v>2015-11-12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2015-11-08</c:v>
+                  <c:v>2015-11-13</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2015-11-09</c:v>
+                  <c:v>2015-11-14</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2015-11-10</c:v>
+                  <c:v>2015-11-15</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2015-11-11</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2015-11-12</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2015-11-13</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2015-11-14</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2015-11-15</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>2015-11-16</c:v>
                 </c:pt>
               </c:strCache>
@@ -2213,9 +2003,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>207_G_drive_load!$B$2:$AG$2</c:f>
+              <c:f>207_G_drive_load!$B$2:$AB$2</c:f>
               <c:numCache>
-                <c:ptCount val="32"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>449.14</c:v>
                 </c:pt>
@@ -2226,10 +2016,10 @@
                   <c:v>449.14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>449.14</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>449.14</c:v>
+                  <c:v>-</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>449.14</c:v>
@@ -2241,10 +2031,10 @@
                   <c:v>449.14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-</c:v>
+                  <c:v>449.14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-</c:v>
+                  <c:v>449.14</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>449.14</c:v>
@@ -2295,21 +2085,6 @@
                   <c:v>449.14</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>449.14</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>449.14</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>449.14</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>449.14</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>449.14</c:v>
-                </c:pt>
-                <c:pt idx="31">
                   <c:v>449.14</c:v>
                 </c:pt>
               </c:numCache>
@@ -2457,100 +2232,85 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>207_Ping!$B$1:$AF$1</c:f>
+              <c:f>207_Ping!$B$1:$AA$1</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>2015-10-17</c:v>
+                  <c:v>2015-10-22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2015-10-18</c:v>
+                  <c:v>2015-10-23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2015-10-19</c:v>
+                  <c:v>2015-10-24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2015-10-20</c:v>
+                  <c:v>2015-10-25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2015-10-21</c:v>
+                  <c:v>2015-10-26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2015-10-22</c:v>
+                  <c:v>2015-10-27</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2015-10-23</c:v>
+                  <c:v>2015-10-28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2015-10-24</c:v>
+                  <c:v>2015-10-29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2015-10-25</c:v>
+                  <c:v>2015-10-30</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2015-10-26</c:v>
+                  <c:v>2015-10-31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2015-10-27</c:v>
+                  <c:v>2015-11-01</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2015-10-28</c:v>
+                  <c:v>2015-11-02</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2015-10-29</c:v>
+                  <c:v>2015-11-03</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2015-10-30</c:v>
+                  <c:v>2015-11-04</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2015-10-31</c:v>
+                  <c:v>2015-11-05</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2015-11-01</c:v>
+                  <c:v>2015-11-06</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2015-11-02</c:v>
+                  <c:v>2015-11-07</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2015-11-03</c:v>
+                  <c:v>2015-11-08</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2015-11-04</c:v>
+                  <c:v>2015-11-09</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2015-11-05</c:v>
+                  <c:v>2015-11-10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2015-11-06</c:v>
+                  <c:v>2015-11-11</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2015-11-07</c:v>
+                  <c:v>2015-11-12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2015-11-08</c:v>
+                  <c:v>2015-11-13</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2015-11-09</c:v>
+                  <c:v>2015-11-14</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2015-11-10</c:v>
+                  <c:v>2015-11-15</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2015-11-11</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2015-11-12</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2015-11-13</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2015-11-14</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2015-11-15</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>2015-11-16</c:v>
                 </c:pt>
               </c:strCache>
@@ -2558,103 +2318,88 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>207_Ping!$B$2:$AG$2</c:f>
+              <c:f>207_Ping!$B$2:$AB$2</c:f>
               <c:numCache>
-                <c:ptCount val="32"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.58</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.48</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>0.42</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.47</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.44</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="17">
                   <c:v>0.42</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.49</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>13.99</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.59</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.52</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.58</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>0.48</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.62</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.53</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.44</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.46</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.46</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.42</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.42</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0.43</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.42</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.46</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.41</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.48</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.43</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.44</c:v>
-                </c:pt>
-                <c:pt idx="31">
                   <c:v>0.42</c:v>
                 </c:pt>
               </c:numCache>
@@ -2756,7 +2501,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -2793,7 +2538,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -2830,7 +2575,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -2867,7 +2612,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -2904,7 +2649,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -2941,7 +2686,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -3258,7 +3003,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -3294,15 +3039,10 @@
     <col min="26" max="26" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="28" max="28" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="30" max="30" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="31" max="31" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="32" max="32" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="33" max="33" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="34" max="34" width="9.10" bestFit="true" style="0"/>
+    <col min="29" max="29" width="9.10" bestFit="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3387,120 +3127,90 @@
       <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="B2">
+        <v>1.73</v>
+      </c>
+      <c r="C2">
+        <v>1.34</v>
+      </c>
+      <c r="D2">
+        <v>1.4</v>
+      </c>
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2">
-        <v>1.28</v>
-      </c>
-      <c r="C2">
-        <v>1.72</v>
-      </c>
-      <c r="D2">
-        <v>1.71</v>
-      </c>
-      <c r="E2">
-        <v>1.88</v>
-      </c>
-      <c r="F2">
-        <v>2.43</v>
+      <c r="F2" t="s">
+        <v>29</v>
       </c>
       <c r="G2">
-        <v>1.73</v>
+        <v>1.09</v>
       </c>
       <c r="H2">
-        <v>1.34</v>
+        <v>0.22</v>
       </c>
       <c r="I2">
-        <v>1.4</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" t="s">
-        <v>34</v>
+        <v>0.84</v>
+      </c>
+      <c r="J2">
+        <v>0.11</v>
+      </c>
+      <c r="K2">
+        <v>0.13</v>
       </c>
       <c r="L2">
-        <v>1.09</v>
+        <v>0.26</v>
       </c>
       <c r="M2">
-        <v>0.22</v>
+        <v>0.32</v>
       </c>
       <c r="N2">
-        <v>0.84</v>
+        <v>0.31</v>
       </c>
       <c r="O2">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="P2">
-        <v>0.13</v>
+        <v>0.08</v>
       </c>
       <c r="Q2">
-        <v>0.26</v>
+        <v>0.1</v>
       </c>
       <c r="R2">
-        <v>0.32</v>
+        <v>0.08</v>
       </c>
       <c r="S2">
-        <v>0.31</v>
+        <v>0.27</v>
       </c>
       <c r="T2">
-        <v>0.1</v>
+        <v>0.29</v>
       </c>
       <c r="U2">
-        <v>0.08</v>
+        <v>0.48</v>
       </c>
       <c r="V2">
-        <v>0.1</v>
+        <v>0.96</v>
       </c>
       <c r="W2">
-        <v>0.08</v>
+        <v>0.95</v>
       </c>
       <c r="X2">
-        <v>0.27</v>
+        <v>0.93</v>
       </c>
       <c r="Y2">
-        <v>0.29</v>
+        <v>1</v>
       </c>
       <c r="Z2">
-        <v>0.48</v>
+        <v>0.93</v>
       </c>
       <c r="AA2">
-        <v>0.96</v>
+        <v>1.04</v>
       </c>
       <c r="AB2">
-        <v>0.95</v>
-      </c>
-      <c r="AC2">
-        <v>0.93</v>
-      </c>
-      <c r="AD2">
-        <v>1</v>
-      </c>
-      <c r="AE2">
-        <v>0.93</v>
-      </c>
-      <c r="AF2">
-        <v>1.04</v>
-      </c>
-      <c r="AG2">
         <v>1.01</v>
       </c>
     </row>
@@ -3526,7 +3236,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -3562,15 +3272,10 @@
     <col min="26" max="26" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="28" max="28" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="30" max="30" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="31" max="31" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="32" max="32" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="33" max="33" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="34" max="34" width="9.10" bestFit="true" style="0"/>
+    <col min="29" max="29" width="9.10" bestFit="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3655,126 +3360,96 @@
       <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>3855.54</v>
+      </c>
+      <c r="C2">
+        <v>3859.14</v>
+      </c>
+      <c r="D2">
+        <v>3853.44</v>
+      </c>
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>2358.98</v>
+      </c>
+      <c r="H2">
+        <v>2600.11</v>
+      </c>
+      <c r="I2">
+        <v>2706</v>
+      </c>
+      <c r="J2">
+        <v>2915.29</v>
+      </c>
+      <c r="K2">
+        <v>2891.85</v>
+      </c>
+      <c r="L2">
+        <v>2836.31</v>
+      </c>
+      <c r="M2">
+        <v>2850.1</v>
+      </c>
+      <c r="N2">
+        <v>2903.58</v>
+      </c>
+      <c r="O2">
+        <v>3070.18</v>
+      </c>
+      <c r="P2">
+        <v>3111.38</v>
+      </c>
+      <c r="Q2">
+        <v>3130.37</v>
+      </c>
+      <c r="R2">
+        <v>3106.2</v>
+      </c>
+      <c r="S2">
+        <v>3085.24</v>
+      </c>
+      <c r="T2">
+        <v>3110.04</v>
+      </c>
+      <c r="U2">
+        <v>3166.98</v>
+      </c>
+      <c r="V2">
+        <v>3263.5</v>
+      </c>
+      <c r="W2">
+        <v>3103.79</v>
+      </c>
+      <c r="X2">
+        <v>3069.64</v>
+      </c>
+      <c r="Y2">
+        <v>3067.38</v>
+      </c>
+      <c r="Z2">
+        <v>3034.69</v>
+      </c>
+      <c r="AA2">
+        <v>3045.34</v>
+      </c>
+      <c r="AB2">
+        <v>3109.32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
+      <c r="A3" t="s">
         <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2">
-        <v>3777.41</v>
-      </c>
-      <c r="C2">
-        <v>3785.78</v>
-      </c>
-      <c r="D2">
-        <v>3786.86</v>
-      </c>
-      <c r="E2">
-        <v>3842.37</v>
-      </c>
-      <c r="F2">
-        <v>3860.83</v>
-      </c>
-      <c r="G2">
-        <v>3855.54</v>
-      </c>
-      <c r="H2">
-        <v>3859.14</v>
-      </c>
-      <c r="I2">
-        <v>3853.44</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2">
-        <v>2358.98</v>
-      </c>
-      <c r="M2">
-        <v>2600.11</v>
-      </c>
-      <c r="N2">
-        <v>2706</v>
-      </c>
-      <c r="O2">
-        <v>2915.29</v>
-      </c>
-      <c r="P2">
-        <v>2891.85</v>
-      </c>
-      <c r="Q2">
-        <v>2836.31</v>
-      </c>
-      <c r="R2">
-        <v>2850.1</v>
-      </c>
-      <c r="S2">
-        <v>2903.58</v>
-      </c>
-      <c r="T2">
-        <v>3070.18</v>
-      </c>
-      <c r="U2">
-        <v>3111.38</v>
-      </c>
-      <c r="V2">
-        <v>3130.37</v>
-      </c>
-      <c r="W2">
-        <v>3106.2</v>
-      </c>
-      <c r="X2">
-        <v>3085.24</v>
-      </c>
-      <c r="Y2">
-        <v>3110.04</v>
-      </c>
-      <c r="Z2">
-        <v>3166.98</v>
-      </c>
-      <c r="AA2">
-        <v>3263.5</v>
-      </c>
-      <c r="AB2">
-        <v>3103.79</v>
-      </c>
-      <c r="AC2">
-        <v>3069.64</v>
-      </c>
-      <c r="AD2">
-        <v>3067.38</v>
-      </c>
-      <c r="AE2">
-        <v>3034.69</v>
-      </c>
-      <c r="AF2">
-        <v>3045.34</v>
-      </c>
-      <c r="AG2">
-        <v>3109.32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34">
-      <c r="A3" t="s">
-        <v>36</v>
       </c>
       <c r="B3">
         <v>8345.09</v>
@@ -3785,11 +3460,11 @@
       <c r="D3">
         <v>8345.09</v>
       </c>
-      <c r="E3">
-        <v>8345.09</v>
-      </c>
-      <c r="F3">
-        <v>8345.09</v>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
       </c>
       <c r="G3">
         <v>8345.09</v>
@@ -3800,11 +3475,11 @@
       <c r="I3">
         <v>8345.09</v>
       </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" t="s">
-        <v>34</v>
+      <c r="J3">
+        <v>8345.09</v>
+      </c>
+      <c r="K3">
+        <v>8345.09</v>
       </c>
       <c r="L3">
         <v>8345.09</v>
@@ -3855,21 +3530,6 @@
         <v>8345.09</v>
       </c>
       <c r="AB3">
-        <v>8345.09</v>
-      </c>
-      <c r="AC3">
-        <v>8345.09</v>
-      </c>
-      <c r="AD3">
-        <v>8345.09</v>
-      </c>
-      <c r="AE3">
-        <v>8345.09</v>
-      </c>
-      <c r="AF3">
-        <v>8345.09</v>
-      </c>
-      <c r="AG3">
         <v>8345.09</v>
       </c>
     </row>
@@ -3895,7 +3555,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -3931,15 +3591,10 @@
     <col min="26" max="26" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="28" max="28" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="30" max="30" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="31" max="31" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="32" max="32" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="33" max="33" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="34" max="34" width="9.10" bestFit="true" style="0"/>
+    <col min="29" max="29" width="9.10" bestFit="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4024,126 +3679,96 @@
       <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>53.63</v>
+      </c>
+      <c r="C2">
+        <v>53.63</v>
+      </c>
+      <c r="D2">
+        <v>53.48</v>
+      </c>
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>53.22</v>
+      </c>
+      <c r="H2">
+        <v>53.19</v>
+      </c>
+      <c r="I2">
+        <v>53.24</v>
+      </c>
+      <c r="J2">
+        <v>53.2</v>
+      </c>
+      <c r="K2">
+        <v>53.13</v>
+      </c>
+      <c r="L2">
+        <v>53.13</v>
+      </c>
+      <c r="M2">
+        <v>53.13</v>
+      </c>
+      <c r="N2">
+        <v>53.13</v>
+      </c>
+      <c r="O2">
+        <v>53.13</v>
+      </c>
+      <c r="P2">
+        <v>53.15</v>
+      </c>
+      <c r="Q2">
+        <v>53.05</v>
+      </c>
+      <c r="R2">
+        <v>52.98</v>
+      </c>
+      <c r="S2">
+        <v>52.98</v>
+      </c>
+      <c r="T2">
+        <v>52.98</v>
+      </c>
+      <c r="U2">
+        <v>52.84</v>
+      </c>
+      <c r="V2">
+        <v>53.01</v>
+      </c>
+      <c r="W2">
+        <v>53.16</v>
+      </c>
+      <c r="X2">
+        <v>53.17</v>
+      </c>
+      <c r="Y2">
+        <v>53.13</v>
+      </c>
+      <c r="Z2">
+        <v>53.08</v>
+      </c>
+      <c r="AA2">
+        <v>53.09</v>
+      </c>
+      <c r="AB2">
+        <v>53.1</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2">
-        <v>53.7</v>
-      </c>
-      <c r="C2">
-        <v>53.61</v>
-      </c>
-      <c r="D2">
-        <v>53.6</v>
-      </c>
-      <c r="E2">
-        <v>53.6</v>
-      </c>
-      <c r="F2">
-        <v>53.62</v>
-      </c>
-      <c r="G2">
-        <v>53.63</v>
-      </c>
-      <c r="H2">
-        <v>53.63</v>
-      </c>
-      <c r="I2">
-        <v>53.48</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2">
-        <v>53.22</v>
-      </c>
-      <c r="M2">
-        <v>53.19</v>
-      </c>
-      <c r="N2">
-        <v>53.24</v>
-      </c>
-      <c r="O2">
-        <v>53.2</v>
-      </c>
-      <c r="P2">
-        <v>53.13</v>
-      </c>
-      <c r="Q2">
-        <v>53.13</v>
-      </c>
-      <c r="R2">
-        <v>53.13</v>
-      </c>
-      <c r="S2">
-        <v>53.13</v>
-      </c>
-      <c r="T2">
-        <v>53.13</v>
-      </c>
-      <c r="U2">
-        <v>53.15</v>
-      </c>
-      <c r="V2">
-        <v>53.05</v>
-      </c>
-      <c r="W2">
-        <v>52.98</v>
-      </c>
-      <c r="X2">
-        <v>52.98</v>
-      </c>
-      <c r="Y2">
-        <v>52.98</v>
-      </c>
-      <c r="Z2">
-        <v>52.84</v>
-      </c>
-      <c r="AA2">
-        <v>53.01</v>
-      </c>
-      <c r="AB2">
-        <v>53.16</v>
-      </c>
-      <c r="AC2">
-        <v>53.17</v>
-      </c>
-      <c r="AD2">
-        <v>53.13</v>
-      </c>
-      <c r="AE2">
-        <v>53.08</v>
-      </c>
-      <c r="AF2">
-        <v>53.09</v>
-      </c>
-      <c r="AG2">
-        <v>53.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>97.3</v>
@@ -4154,11 +3779,11 @@
       <c r="D3">
         <v>97.3</v>
       </c>
-      <c r="E3">
-        <v>97.3</v>
-      </c>
-      <c r="F3">
-        <v>97.3</v>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
       </c>
       <c r="G3">
         <v>97.3</v>
@@ -4169,11 +3794,11 @@
       <c r="I3">
         <v>97.3</v>
       </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" t="s">
-        <v>34</v>
+      <c r="J3">
+        <v>97.3</v>
+      </c>
+      <c r="K3">
+        <v>97.3</v>
       </c>
       <c r="L3">
         <v>97.3</v>
@@ -4224,21 +3849,6 @@
         <v>97.3</v>
       </c>
       <c r="AB3">
-        <v>97.3</v>
-      </c>
-      <c r="AC3">
-        <v>97.3</v>
-      </c>
-      <c r="AD3">
-        <v>97.3</v>
-      </c>
-      <c r="AE3">
-        <v>97.3</v>
-      </c>
-      <c r="AF3">
-        <v>97.3</v>
-      </c>
-      <c r="AG3">
         <v>97.3</v>
       </c>
     </row>
@@ -4264,7 +3874,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -4300,15 +3910,10 @@
     <col min="26" max="26" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="28" max="28" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="30" max="30" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="31" max="31" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="32" max="32" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="33" max="33" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="34" max="34" width="9.10" bestFit="true" style="0"/>
+    <col min="29" max="29" width="9.10" bestFit="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4393,25 +3998,10 @@
       <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34">
-      <c r="A2" t="s">
-        <v>37</v>
       </c>
       <c r="B2">
         <v>446.38</v>
@@ -4422,11 +4012,11 @@
       <c r="D2">
         <v>446.38</v>
       </c>
-      <c r="E2">
-        <v>446.38</v>
-      </c>
-      <c r="F2">
-        <v>446.38</v>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
       </c>
       <c r="G2">
         <v>446.38</v>
@@ -4437,11 +4027,11 @@
       <c r="I2">
         <v>446.38</v>
       </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" t="s">
-        <v>34</v>
+      <c r="J2">
+        <v>446.38</v>
+      </c>
+      <c r="K2">
+        <v>446.38</v>
       </c>
       <c r="L2">
         <v>446.38</v>
@@ -4494,25 +4084,10 @@
       <c r="AB2">
         <v>446.38</v>
       </c>
-      <c r="AC2">
-        <v>446.38</v>
-      </c>
-      <c r="AD2">
-        <v>446.38</v>
-      </c>
-      <c r="AE2">
-        <v>446.38</v>
-      </c>
-      <c r="AF2">
-        <v>446.38</v>
-      </c>
-      <c r="AG2">
-        <v>446.38</v>
-      </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>461.43</v>
@@ -4523,11 +4098,11 @@
       <c r="D3">
         <v>461.43</v>
       </c>
-      <c r="E3">
-        <v>461.43</v>
-      </c>
-      <c r="F3">
-        <v>461.43</v>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
       </c>
       <c r="G3">
         <v>461.43</v>
@@ -4538,11 +4113,11 @@
       <c r="I3">
         <v>461.43</v>
       </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" t="s">
-        <v>34</v>
+      <c r="J3">
+        <v>461.43</v>
+      </c>
+      <c r="K3">
+        <v>461.43</v>
       </c>
       <c r="L3">
         <v>461.43</v>
@@ -4593,21 +4168,6 @@
         <v>461.43</v>
       </c>
       <c r="AB3">
-        <v>461.43</v>
-      </c>
-      <c r="AC3">
-        <v>461.43</v>
-      </c>
-      <c r="AD3">
-        <v>461.43</v>
-      </c>
-      <c r="AE3">
-        <v>461.43</v>
-      </c>
-      <c r="AF3">
-        <v>461.43</v>
-      </c>
-      <c r="AG3">
         <v>461.43</v>
       </c>
     </row>
@@ -4633,7 +4193,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -4669,15 +4229,10 @@
     <col min="26" max="26" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="28" max="28" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="30" max="30" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="31" max="31" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="32" max="32" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="33" max="33" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="34" max="34" width="9.10" bestFit="true" style="0"/>
+    <col min="29" max="29" width="9.10" bestFit="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4762,25 +4317,10 @@
       <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34">
-      <c r="A2" t="s">
-        <v>37</v>
       </c>
       <c r="B2">
         <v>449.14</v>
@@ -4791,11 +4331,11 @@
       <c r="D2">
         <v>449.14</v>
       </c>
-      <c r="E2">
-        <v>449.14</v>
-      </c>
-      <c r="F2">
-        <v>449.14</v>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
       </c>
       <c r="G2">
         <v>449.14</v>
@@ -4806,11 +4346,11 @@
       <c r="I2">
         <v>449.14</v>
       </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" t="s">
-        <v>34</v>
+      <c r="J2">
+        <v>449.14</v>
+      </c>
+      <c r="K2">
+        <v>449.14</v>
       </c>
       <c r="L2">
         <v>449.14</v>
@@ -4863,25 +4403,10 @@
       <c r="AB2">
         <v>449.14</v>
       </c>
-      <c r="AC2">
-        <v>449.14</v>
-      </c>
-      <c r="AD2">
-        <v>449.14</v>
-      </c>
-      <c r="AE2">
-        <v>449.14</v>
-      </c>
-      <c r="AF2">
-        <v>449.14</v>
-      </c>
-      <c r="AG2">
-        <v>449.14</v>
-      </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>1117.76</v>
@@ -4892,11 +4417,11 @@
       <c r="D3">
         <v>1117.76</v>
       </c>
-      <c r="E3">
-        <v>1117.76</v>
-      </c>
-      <c r="F3">
-        <v>1117.76</v>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
       </c>
       <c r="G3">
         <v>1117.76</v>
@@ -4907,11 +4432,11 @@
       <c r="I3">
         <v>1117.76</v>
       </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" t="s">
-        <v>34</v>
+      <c r="J3">
+        <v>1117.76</v>
+      </c>
+      <c r="K3">
+        <v>1117.76</v>
       </c>
       <c r="L3">
         <v>1117.76</v>
@@ -4962,21 +4487,6 @@
         <v>1117.76</v>
       </c>
       <c r="AB3">
-        <v>1117.76</v>
-      </c>
-      <c r="AC3">
-        <v>1117.76</v>
-      </c>
-      <c r="AD3">
-        <v>1117.76</v>
-      </c>
-      <c r="AE3">
-        <v>1117.76</v>
-      </c>
-      <c r="AF3">
-        <v>1117.76</v>
-      </c>
-      <c r="AG3">
         <v>1117.76</v>
       </c>
     </row>
@@ -5002,7 +4512,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -5038,15 +4548,10 @@
     <col min="26" max="26" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="28" max="28" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="30" max="30" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="31" max="31" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="32" max="32" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="33" max="33" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="34" max="34" width="9.10" bestFit="true" style="0"/>
+    <col min="29" max="29" width="9.10" bestFit="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5131,120 +4636,90 @@
       <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>0.42</v>
+      </c>
+      <c r="C2">
+        <v>0.49</v>
+      </c>
+      <c r="D2">
+        <v>13.99</v>
+      </c>
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2">
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>0.65</v>
+      </c>
+      <c r="H2">
+        <v>0.6</v>
+      </c>
+      <c r="I2">
+        <v>0.59</v>
+      </c>
+      <c r="J2">
+        <v>0.52</v>
+      </c>
+      <c r="K2">
+        <v>0.58</v>
+      </c>
+      <c r="L2">
         <v>0.48</v>
       </c>
-      <c r="C2">
+      <c r="M2">
+        <v>0.62</v>
+      </c>
+      <c r="N2">
+        <v>0.53</v>
+      </c>
+      <c r="O2">
+        <v>0.44</v>
+      </c>
+      <c r="P2">
+        <v>0.46</v>
+      </c>
+      <c r="Q2">
+        <v>0.46</v>
+      </c>
+      <c r="R2">
         <v>0.42</v>
       </c>
-      <c r="D2">
-        <v>0.45</v>
-      </c>
-      <c r="E2">
-        <v>0.47</v>
-      </c>
-      <c r="F2">
-        <v>0.44</v>
-      </c>
-      <c r="G2">
+      <c r="S2">
         <v>0.42</v>
       </c>
-      <c r="H2">
-        <v>0.49</v>
-      </c>
-      <c r="I2">
-        <v>13.99</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2">
-        <v>0.65</v>
-      </c>
-      <c r="M2">
-        <v>0.6</v>
-      </c>
-      <c r="N2">
-        <v>0.59</v>
-      </c>
-      <c r="O2">
-        <v>0.52</v>
-      </c>
-      <c r="P2">
-        <v>0.58</v>
-      </c>
-      <c r="Q2">
+      <c r="T2">
+        <v>0.4</v>
+      </c>
+      <c r="U2">
+        <v>0.43</v>
+      </c>
+      <c r="V2">
+        <v>0.42</v>
+      </c>
+      <c r="W2">
+        <v>0.46</v>
+      </c>
+      <c r="X2">
+        <v>0.41</v>
+      </c>
+      <c r="Y2">
         <v>0.48</v>
-      </c>
-      <c r="R2">
-        <v>0.62</v>
-      </c>
-      <c r="S2">
-        <v>0.53</v>
-      </c>
-      <c r="T2">
-        <v>0.44</v>
-      </c>
-      <c r="U2">
-        <v>0.46</v>
-      </c>
-      <c r="V2">
-        <v>0.46</v>
-      </c>
-      <c r="W2">
-        <v>0.42</v>
-      </c>
-      <c r="X2">
-        <v>0.42</v>
-      </c>
-      <c r="Y2">
-        <v>0.4</v>
       </c>
       <c r="Z2">
         <v>0.43</v>
       </c>
       <c r="AA2">
-        <v>0.42</v>
+        <v>0.44</v>
       </c>
       <c r="AB2">
-        <v>0.46</v>
-      </c>
-      <c r="AC2">
-        <v>0.41</v>
-      </c>
-      <c r="AD2">
-        <v>0.48</v>
-      </c>
-      <c r="AE2">
-        <v>0.43</v>
-      </c>
-      <c r="AF2">
-        <v>0.44</v>
-      </c>
-      <c r="AG2">
         <v>0.42</v>
       </c>
     </row>

</xml_diff>